<commit_message>
add not pass reason
</commit_message>
<xml_diff>
--- a/doc/other/山东省企业名录.xlsx
+++ b/doc/other/山东省企业名录.xlsx
@@ -18798,51 +18798,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>355</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2876550</xdr:colOff>
-      <xdr:row>365</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="60874275"/>
-          <a:ext cx="2876550" cy="1714500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19134,7 +19089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1567"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -50497,7 +50452,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
-  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>